<commit_message>
added webscraping materials and updated buble plot with time slider and animations
</commit_message>
<xml_diff>
--- a/artifacts/datasets/business_of_apps_Netflix.xlsx
+++ b/artifacts/datasets/business_of_apps_Netflix.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaor\OneDrive\Desktop\git hub projects\data_vis\D-D-D-Data-Dazzlers\artifacts\datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD14F81F-122B-4D77-8C85-384DAEEA6B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Netflix annual revenue" sheetId="1" r:id="rId1"/>
-    <sheet name="Netflix revenue by region" sheetId="2" r:id="rId2"/>
+    <sheet name=" Netflix revenue by region ($bn" sheetId="2" r:id="rId2"/>
     <sheet name="Netflix ARPU by region" sheetId="3" r:id="rId3"/>
-    <sheet name="Netflix net income" sheetId="4" r:id="rId4"/>
+    <sheet name="Net income or loss" sheetId="4" r:id="rId4"/>
     <sheet name="Netflix annual content spend" sheetId="5" r:id="rId5"/>
     <sheet name="Netflix annual subscribers" sheetId="6" r:id="rId6"/>
     <sheet name="Netflix subscribers by region" sheetId="7" r:id="rId7"/>
@@ -18,12 +24,12 @@
     <sheet name="Netflix share of streaming minu" sheetId="9" r:id="rId9"/>
     <sheet name="US streaming content library si" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="192">
   <si>
     <t>Year</t>
   </si>
@@ -596,13 +602,16 @@
   </si>
   <si>
     <t>50</t>
+  </si>
+  <si>
+    <t>ARPU = average revenue per user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,9 +663,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -665,13 +677,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -709,7 +729,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -743,6 +763,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -777,9 +798,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -952,14 +974,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -975,7 +999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -983,7 +1007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -991,7 +1015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +1039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1047,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1039,7 +1063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1047,7 +1071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1055,7 +1079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1063,7 +1087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1071,7 +1095,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1085,14 +1109,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
@@ -1103,7 +1127,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -1114,7 +1138,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -1125,7 +1149,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>174</v>
       </c>
@@ -1136,7 +1160,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -1147,7 +1171,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -1158,7 +1182,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>175</v>
       </c>
@@ -1169,7 +1193,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>176</v>
       </c>
@@ -1180,7 +1204,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -1197,14 +1221,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1247,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1238,7 +1264,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1255,7 +1281,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1272,7 +1298,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1289,7 +1315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1306,7 +1332,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1323,7 +1349,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1346,14 +1372,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="31.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1369,8 +1400,11 @@
       <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="H1" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1387,7 +1421,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1404,7 +1438,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1421,7 +1455,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1438,7 +1472,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1489,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1472,7 +1506,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1495,14 +1529,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1546,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1554,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1526,7 +1562,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1534,7 +1570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1542,7 +1578,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1550,7 +1586,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1594,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1566,7 +1602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1610,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1582,7 +1618,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1590,7 +1626,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1598,7 +1634,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1606,7 +1642,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1650,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1628,14 +1664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1679,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1651,7 +1687,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1659,7 +1695,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1667,7 +1703,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1675,7 +1711,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1683,7 +1719,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1691,7 +1727,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1699,7 +1735,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1707,7 +1743,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1721,14 +1757,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>113</v>
       </c>
@@ -1736,7 +1772,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1744,7 +1780,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1752,7 +1788,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1760,7 +1796,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1768,7 +1804,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1776,7 +1812,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1784,7 +1820,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1792,7 +1828,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1800,7 +1836,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1808,7 +1844,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1816,7 +1852,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1824,7 +1860,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1832,7 +1868,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1840,7 +1876,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1854,14 +1890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +1914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1895,7 +1931,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1912,7 +1948,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1929,7 +1965,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1946,7 +1982,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1963,7 +1999,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1980,7 +2016,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2003,14 +2039,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>113</v>
       </c>
@@ -2018,7 +2054,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2026,7 +2062,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2040,14 +2076,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
@@ -2055,7 +2091,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -2063,7 +2099,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>162</v>
       </c>
@@ -2071,7 +2107,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -2079,7 +2115,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -2087,7 +2123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -2095,7 +2131,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>166</v>
       </c>

</xml_diff>